<commit_message>
This will be the longest  version of the presentation. In the following commits, I will reduce the speaking time to 10 minutes.
</commit_message>
<xml_diff>
--- a/Excel_References.xlsx
+++ b/Excel_References.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28019"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28020"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/ennowinkler_ennosgermancourse_onmicrosoft_com/Documents/PhDProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1074" documentId="13_ncr:1_{92D5FB84-227A-4306-9187-93183921DEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04835E10-BD13-4F7C-A0C0-0B70461E9250}"/>
+  <xr:revisionPtr revIDLastSave="1097" documentId="13_ncr:1_{92D5FB84-227A-4306-9187-93183921DEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC8C99B5-3A4A-43D4-861C-F9850FA32004}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5460" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="270">
   <si>
     <t xml:space="preserve">@INCOLLECTION{Mauss2009-uk,   title = {Culture and automatic emotion regulation},   booktitle = {Regulating Emotions},   author = {Mauss, Iris B and Bunge, Silvia A and Gross, James J},   publisher = {Blackwell Publishing Ltd.},   pages = {39--60},   year = 2009,   address = {Oxford, UK} }  </t>
   </si>
@@ -1122,6 +1122,9 @@
     <t>Predoc</t>
   </si>
   <si>
+    <t>https://ennosgermancourse-my.sharepoint.com/:b:/g/personal/ennowinkler_ennosgermancourse_onmicrosoft_com/EX6Sh59ie2tGh-rJ74UShvABIwiXky4HvT00IylWAaKDxw?e=CjMXIn</t>
+  </si>
+  <si>
     <t>@article{Eid2001,
   title = {Norms for experiencing emotions in different cultures: Inter- and intranational differences.},
   volume = {81},
@@ -1544,6 +1547,62 @@
   year = {1983},
   volume = {13},
   number = {1-2}
+}</t>
+  </si>
+  <si>
+    <t>@article{Fredrickson2004,
+  title = {The broaden–and–build theory of positive emotions},
+  volume = {359},
+  ISSN = {1471-2970},
+  url = {http://dx.doi.org/10.1098/rstb.2004.1512},
+  DOI = {10.1098/rstb.2004.1512},
+  number = {1449},
+  journal = {Philosophical Transactions of the Royal Society of London. Series B: Biological Sciences},
+  publisher = {The Royal Society},
+  author = {Fredrickson,  Barbara L.},
+  editor = {Huppert,  F. A. and Baylis,  N. and Keverne,  B.},
+  year = {2004},
+  month = sep,
+  pages = {1367–1377}
+}</t>
+  </si>
+  <si>
+    <t>@article{Tang2020,
+  author = {Mary Tang},
+  title = {‘Awe’some Choice: An Expansion of the Broaden and Build Theory},
+  journal = {BSU Honors Program Theses and Projects},
+  year = {2020},
+  number = {Item 346},
+  url = {https://vc.bridgew.edu/honors_proj/346},
+}</t>
+  </si>
+  <si>
+    <t>https://ennosgermancourse-my.sharepoint.com/:b:/g/personal/ennowinkler_ennosgermancourse_onmicrosoft_com/EUZhYJV-ovZBpX21IDEqqBsBBW1WYlNlXGzeuvVg0AZjLw?e=bzOfXv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@incollection{Smith2014,
+  author = {C. A. Smith and E. M. Tong and P. C. Ellsworth},
+  title = {The differentiation of positive emotional experience as viewed through the lens of appraisal theory},
+  booktitle = {The Handbook of Positive Emotions},
+  editor = {M. Tugade and M. Shiota and L. D. Kirby},
+  pages = {11--27},
+  publisher = {Guilford},
+  year = {2014},
+}
+</t>
+  </si>
+  <si>
+    <t>https://ennosgermancourse-my.sharepoint.com/:b:/g/personal/ennowinkler_ennosgermancourse_onmicrosoft_com/EZvjpTYvN0lOpknuAoBR_7AB27iKVWM1zRqb2ahrga7EzA?e=b9niA7</t>
+  </si>
+  <si>
+    <t>Emotions are different from person to person</t>
+  </si>
+  <si>
+    <t>@book{tiberius2018well,
+  title = {Well-being as value fulfillment: How we can help each other to live well},
+  author = {Tiberius, Valerie},
+  year = {2018},
+  publisher = {Oxford University Press, USA}
 }</t>
   </si>
   <si>
@@ -19622,8 +19681,8 @@
   <dimension ref="A1:S508"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -21695,7 +21754,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" ht="52.5">
+    <row r="53" spans="1:11" ht="121.5">
       <c r="A53" s="54" t="s">
         <v>128</v>
       </c>
@@ -21731,11 +21790,13 @@
         <v>129</v>
       </c>
       <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
+      <c r="K53" s="43" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="54" spans="1:11" ht="52.5">
       <c r="A54" s="54" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B54" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21773,7 +21834,7 @@
     </row>
     <row r="55" spans="1:11" ht="52.5">
       <c r="A55" s="54" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B55" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21811,7 +21872,7 @@
     </row>
     <row r="56" spans="1:11" ht="63">
       <c r="A56" s="55" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B56" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21849,7 +21910,7 @@
     </row>
     <row r="57" spans="1:11" ht="52.5">
       <c r="A57" s="54" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B57" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21887,7 +21948,7 @@
     </row>
     <row r="58" spans="1:11" ht="63">
       <c r="A58" s="54" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B58" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21925,7 +21986,7 @@
     </row>
     <row r="59" spans="1:11" ht="42">
       <c r="A59" s="54" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B59" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21963,7 +22024,7 @@
     </row>
     <row r="60" spans="1:11" ht="52.5">
       <c r="A60" s="54" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B60" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22001,7 +22062,7 @@
     </row>
     <row r="61" spans="1:11" ht="33.75">
       <c r="A61" s="56" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B61" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22038,7 +22099,7 @@
     </row>
     <row r="62" spans="1:11" ht="52.5">
       <c r="A62" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B62" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22073,7 +22134,7 @@
     </row>
     <row r="63" spans="1:11" ht="52.5">
       <c r="A63" s="53" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B63" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22108,7 +22169,7 @@
     </row>
     <row r="64" spans="1:11" ht="33.75">
       <c r="A64" s="53" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B64" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22143,7 +22204,7 @@
     </row>
     <row r="65" spans="1:11" ht="52.5">
       <c r="A65" s="53" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B65" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22178,7 +22239,7 @@
     </row>
     <row r="66" spans="1:11" ht="52.5">
       <c r="A66" s="53" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B66" s="62" t="str">
         <f t="shared" ref="B66" si="15">IFERROR("@" &amp; MID(A66, SEARCH("{", A66) + 1, SEARCH(",", A66) - SEARCH("{", A66) - 1), "")</f>
@@ -22213,7 +22274,7 @@
     </row>
     <row r="67" spans="1:11" ht="52.5">
       <c r="A67" s="53" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B67" s="62" t="str">
         <f t="shared" ref="B67" si="22">IFERROR("@" &amp; MID(A67, SEARCH("{", A67) + 1, SEARCH(",", A67) - SEARCH("{", A67) - 1), "")</f>
@@ -22249,7 +22310,7 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B68" s="62" t="str">
         <f t="shared" ref="B68:B69" si="29">IFERROR("@" &amp; MID(A68, SEARCH("{", A68) + 1, SEARCH(",", A68) - SEARCH("{", A68) - 1), "")</f>
@@ -22283,7 +22344,7 @@
     </row>
     <row r="69" spans="1:11" ht="52.5">
       <c r="A69" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B69" s="62" t="str">
         <f t="shared" si="29"/>
@@ -22317,7 +22378,7 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B70" s="62" t="str">
         <f t="shared" ref="B70" si="36">IFERROR("@" &amp; MID(A70, SEARCH("{", A70) + 1, SEARCH(",", A70) - SEARCH("{", A70) - 1), "")</f>
@@ -22348,13 +22409,13 @@
         <v>45458.517281365741</v>
       </c>
       <c r="I70" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K70"/>
     </row>
     <row r="71" spans="1:11" ht="52.5">
       <c r="A71" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B71" s="62" t="str">
         <f t="shared" ref="B71" si="43">IFERROR("@" &amp; MID(A71, SEARCH("{", A71) + 1, SEARCH(",", A71) - SEARCH("{", A71) - 1), "")</f>
@@ -22385,13 +22446,13 @@
         <v>45458.535618402777</v>
       </c>
       <c r="I71" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K71"/>
     </row>
     <row r="72" spans="1:11" ht="63">
       <c r="A72" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B72" s="62" t="str">
         <f t="shared" ref="B72" si="50">IFERROR("@" &amp; MID(A72, SEARCH("{", A72) + 1, SEARCH(",", A72) - SEARCH("{", A72) - 1), "")</f>
@@ -22427,12 +22488,12 @@
         <v>35</v>
       </c>
       <c r="K72" s="42" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B73" s="62" t="str">
         <f t="shared" ref="B73:B83" si="57">IFERROR("@" &amp; MID(A73, SEARCH("{", A73) + 1, SEARCH(",", A73) - SEARCH("{", A73) - 1), "")</f>
@@ -22463,13 +22524,13 @@
         <v>45526.456741666669</v>
       </c>
       <c r="I73" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K73"/>
     </row>
     <row r="74" spans="1:11" ht="180">
       <c r="A74" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B74" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22500,13 +22561,13 @@
         <v>45526.459042361108</v>
       </c>
       <c r="I74" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K74"/>
     </row>
     <row r="75" spans="1:11" ht="195">
       <c r="A75" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B75" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22540,7 +22601,7 @@
     </row>
     <row r="76" spans="1:11" ht="345">
       <c r="A76" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B76" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22577,7 +22638,7 @@
     </row>
     <row r="77" spans="1:11" ht="240">
       <c r="A77" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B77" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22611,7 +22672,7 @@
     </row>
     <row r="78" spans="1:11" ht="240">
       <c r="A78" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B78" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22645,7 +22706,7 @@
     </row>
     <row r="79" spans="1:11" ht="152.25">
       <c r="A79" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B79" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22678,132 +22739,159 @@
       </c>
       <c r="K79"/>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" ht="244.5">
+      <c r="A80" s="4" t="s">
+        <v>161</v>
+      </c>
       <c r="B80" s="62" t="str">
         <f t="shared" si="57"/>
-        <v/>
+        <v>@Fredrickson2004</v>
       </c>
       <c r="C80" s="63" t="str">
         <f t="shared" si="58"/>
-        <v>[]</v>
+        <v>[@Fredrickson2004]</v>
       </c>
       <c r="D80" s="63" t="str">
         <f t="shared" si="59"/>
-        <v/>
+        <v>2004</v>
       </c>
       <c r="E80" s="64" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>Fredrickson,  Barbara L.</v>
       </c>
       <c r="F80" s="65" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>The broaden–and–build theory of positive emotions</v>
       </c>
       <c r="G80" s="66" t="str">
         <f t="shared" si="62"/>
-        <v/>
-      </c>
-      <c r="H80" s="67" t="str">
+        <v>https://doi.org/10.1098/rstb.2004.1512</v>
+      </c>
+      <c r="H80" s="67">
         <f t="shared" ca="1" si="63"/>
-        <v/>
+        <v>45528.482871643515</v>
       </c>
       <c r="K80"/>
     </row>
-    <row r="81" spans="1:8" customFormat="1">
-      <c r="A81" s="3"/>
+    <row r="81" spans="1:18" ht="121.5">
+      <c r="A81" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="B81" s="62" t="str">
         <f t="shared" si="57"/>
-        <v/>
+        <v>@Tang2020</v>
       </c>
       <c r="C81" s="63" t="str">
         <f t="shared" si="58"/>
-        <v>[]</v>
+        <v>[@Tang2020]</v>
       </c>
       <c r="D81" s="63" t="str">
         <f t="shared" si="59"/>
-        <v/>
+        <v>2020</v>
       </c>
       <c r="E81" s="64" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>Mary Tang</v>
       </c>
       <c r="F81" s="65" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>‘Awe’some Choice: An Expansion of the Broaden and Build Theory</v>
       </c>
       <c r="G81" s="66" t="str">
         <f t="shared" si="62"/>
         <v/>
       </c>
-      <c r="H81" s="67" t="str">
+      <c r="H81" s="67">
         <f t="shared" ca="1" si="63"/>
-        <v/>
-      </c>
-    </row>
-    <row r="82" spans="1:8" customFormat="1">
-      <c r="A82" s="3"/>
+        <v>45528.489821759256</v>
+      </c>
+      <c r="I81" t="s">
+        <v>35</v>
+      </c>
+      <c r="J81" t="s">
+        <v>58</v>
+      </c>
+      <c r="K81" s="42" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" ht="167.25">
+      <c r="A82" s="4" t="s">
+        <v>164</v>
+      </c>
       <c r="B82" s="62" t="str">
         <f t="shared" si="57"/>
-        <v/>
+        <v>@Smith2014</v>
       </c>
       <c r="C82" s="63" t="str">
         <f t="shared" si="58"/>
-        <v>[]</v>
+        <v>[@Smith2014]</v>
       </c>
       <c r="D82" s="63" t="str">
         <f t="shared" si="59"/>
-        <v/>
+        <v>2014</v>
       </c>
       <c r="E82" s="64" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>C. A. Smith and E. M. Tong and P. C. Ellsworth</v>
       </c>
       <c r="F82" s="65" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>The differentiation of positive emotional experience as viewed through the lens of appraisal theory</v>
       </c>
       <c r="G82" s="66" t="str">
         <f t="shared" si="62"/>
         <v/>
       </c>
-      <c r="H82" s="67" t="str">
+      <c r="H82" s="67">
         <f t="shared" ca="1" si="63"/>
-        <v/>
-      </c>
-    </row>
-    <row r="83" spans="1:8" customFormat="1">
-      <c r="A83" s="3"/>
+        <v>45528.510834490742</v>
+      </c>
+      <c r="J82" t="s">
+        <v>58</v>
+      </c>
+      <c r="K82" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="R82" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" ht="91.5">
+      <c r="A83" s="4" t="s">
+        <v>167</v>
+      </c>
       <c r="B83" s="62" t="str">
         <f t="shared" si="57"/>
-        <v/>
+        <v>@tiberius2018well</v>
       </c>
       <c r="C83" s="63" t="str">
         <f t="shared" si="58"/>
-        <v>[]</v>
+        <v>[@tiberius2018well]</v>
       </c>
       <c r="D83" s="63" t="str">
         <f t="shared" si="59"/>
-        <v/>
+        <v>2018</v>
       </c>
       <c r="E83" s="64" t="str">
         <f t="shared" si="60"/>
-        <v/>
+        <v>Tiberius, Valerie</v>
       </c>
       <c r="F83" s="65" t="str">
         <f t="shared" si="61"/>
-        <v/>
+        <v>Well-being as value fulfillment: How we can help each other to live well</v>
       </c>
       <c r="G83" s="66" t="str">
         <f t="shared" si="62"/>
         <v/>
       </c>
-      <c r="H83" s="67" t="str">
+      <c r="H83" s="67">
         <f t="shared" ca="1" si="63"/>
-        <v/>
-      </c>
-    </row>
-    <row r="84" spans="1:8" customFormat="1" ht="15">
-      <c r="A84" s="3"/>
+        <v>45528.541320486111</v>
+      </c>
+      <c r="K83"/>
+    </row>
+    <row r="84" spans="1:18" ht="15">
       <c r="B84" s="68"/>
       <c r="C84" s="68"/>
       <c r="D84" s="68"/>
@@ -22811,9 +22899,9 @@
       <c r="F84" s="68"/>
       <c r="G84" s="68"/>
       <c r="H84" s="68"/>
-    </row>
-    <row r="85" spans="1:8" customFormat="1" ht="15">
-      <c r="A85" s="3"/>
+      <c r="K84"/>
+    </row>
+    <row r="85" spans="1:18" ht="15">
       <c r="B85" s="68"/>
       <c r="C85" s="68"/>
       <c r="D85" s="68"/>
@@ -22821,9 +22909,9 @@
       <c r="F85" s="68"/>
       <c r="G85" s="68"/>
       <c r="H85" s="68"/>
-    </row>
-    <row r="86" spans="1:8" customFormat="1" ht="15">
-      <c r="A86" s="3"/>
+      <c r="K85"/>
+    </row>
+    <row r="86" spans="1:18" ht="15">
       <c r="B86" s="68"/>
       <c r="C86" s="68"/>
       <c r="D86" s="68"/>
@@ -22831,9 +22919,9 @@
       <c r="F86" s="68"/>
       <c r="G86" s="68"/>
       <c r="H86" s="68"/>
-    </row>
-    <row r="87" spans="1:8" customFormat="1" ht="15">
-      <c r="A87" s="3"/>
+      <c r="K86"/>
+    </row>
+    <row r="87" spans="1:18" ht="15">
       <c r="B87" s="68"/>
       <c r="C87" s="68"/>
       <c r="D87" s="68"/>
@@ -22841,9 +22929,9 @@
       <c r="F87" s="68"/>
       <c r="G87" s="68"/>
       <c r="H87" s="68"/>
-    </row>
-    <row r="88" spans="1:8" customFormat="1" ht="15">
-      <c r="A88" s="3"/>
+      <c r="K87"/>
+    </row>
+    <row r="88" spans="1:18" ht="15">
       <c r="B88" s="68"/>
       <c r="C88" s="68"/>
       <c r="D88" s="68"/>
@@ -22851,9 +22939,9 @@
       <c r="F88" s="68"/>
       <c r="G88" s="68"/>
       <c r="H88" s="68"/>
-    </row>
-    <row r="89" spans="1:8" customFormat="1" ht="15">
-      <c r="A89" s="3"/>
+      <c r="K88"/>
+    </row>
+    <row r="89" spans="1:18" ht="15">
       <c r="B89" s="68"/>
       <c r="C89" s="68"/>
       <c r="D89" s="68"/>
@@ -22861,9 +22949,9 @@
       <c r="F89" s="68"/>
       <c r="G89" s="68"/>
       <c r="H89" s="68"/>
-    </row>
-    <row r="90" spans="1:8" customFormat="1" ht="15">
-      <c r="A90" s="3"/>
+      <c r="K89"/>
+    </row>
+    <row r="90" spans="1:18" ht="15">
       <c r="B90" s="68"/>
       <c r="C90" s="68"/>
       <c r="D90" s="68"/>
@@ -22871,9 +22959,9 @@
       <c r="F90" s="68"/>
       <c r="G90" s="68"/>
       <c r="H90" s="68"/>
-    </row>
-    <row r="91" spans="1:8" customFormat="1" ht="15">
-      <c r="A91" s="3"/>
+      <c r="K90"/>
+    </row>
+    <row r="91" spans="1:18" ht="15">
       <c r="B91" s="68"/>
       <c r="C91" s="68"/>
       <c r="D91" s="68"/>
@@ -22881,9 +22969,9 @@
       <c r="F91" s="68"/>
       <c r="G91" s="68"/>
       <c r="H91" s="68"/>
-    </row>
-    <row r="92" spans="1:8" customFormat="1" ht="15">
-      <c r="A92" s="3"/>
+      <c r="K91"/>
+    </row>
+    <row r="92" spans="1:18" ht="15">
       <c r="B92" s="68"/>
       <c r="C92" s="68"/>
       <c r="D92" s="68"/>
@@ -22891,9 +22979,9 @@
       <c r="F92" s="68"/>
       <c r="G92" s="68"/>
       <c r="H92" s="68"/>
-    </row>
-    <row r="93" spans="1:8" customFormat="1" ht="15">
-      <c r="A93" s="3"/>
+      <c r="K92"/>
+    </row>
+    <row r="93" spans="1:18" ht="15">
       <c r="B93" s="68"/>
       <c r="C93" s="68"/>
       <c r="D93" s="68"/>
@@ -22901,9 +22989,9 @@
       <c r="F93" s="68"/>
       <c r="G93" s="68"/>
       <c r="H93" s="68"/>
-    </row>
-    <row r="94" spans="1:8" customFormat="1" ht="15">
-      <c r="A94" s="3"/>
+      <c r="K93"/>
+    </row>
+    <row r="94" spans="1:18" ht="15">
       <c r="B94" s="68"/>
       <c r="C94" s="68"/>
       <c r="D94" s="68"/>
@@ -22911,9 +22999,9 @@
       <c r="F94" s="68"/>
       <c r="G94" s="68"/>
       <c r="H94" s="68"/>
-    </row>
-    <row r="95" spans="1:8" customFormat="1" ht="15">
-      <c r="A95" s="3"/>
+      <c r="K94"/>
+    </row>
+    <row r="95" spans="1:18" ht="15">
       <c r="B95" s="68"/>
       <c r="C95" s="68"/>
       <c r="D95" s="68"/>
@@ -22921,9 +23009,9 @@
       <c r="F95" s="68"/>
       <c r="G95" s="68"/>
       <c r="H95" s="68"/>
-    </row>
-    <row r="96" spans="1:8" customFormat="1" ht="15">
-      <c r="A96" s="3"/>
+      <c r="K95"/>
+    </row>
+    <row r="96" spans="1:18" ht="15">
       <c r="B96" s="68"/>
       <c r="C96" s="68"/>
       <c r="D96" s="68"/>
@@ -22931,6 +23019,7 @@
       <c r="F96" s="68"/>
       <c r="G96" s="68"/>
       <c r="H96" s="68"/>
+      <c r="K96"/>
     </row>
     <row r="97" spans="1:8" customFormat="1" ht="15">
       <c r="A97" s="3"/>
@@ -27099,10 +27188,13 @@
     <hyperlink ref="K34" r:id="rId16" xr:uid="{F7A7A198-5E75-4A75-B48A-E95EF1224AF8}"/>
     <hyperlink ref="K72" r:id="rId17" xr:uid="{00985FF8-8F7A-4337-86FD-A8D09F90B6DE}"/>
     <hyperlink ref="K32" r:id="rId18" xr:uid="{3E1D915C-6BEF-4B2B-8143-A3135B742BA8}"/>
+    <hyperlink ref="K81" r:id="rId19" xr:uid="{B9E485E6-BADC-4A83-9974-630741579315}"/>
+    <hyperlink ref="K82" r:id="rId20" xr:uid="{1026A02B-7C1E-42C0-B517-6E308BE4FBCE}"/>
+    <hyperlink ref="K53" r:id="rId21" xr:uid="{85B081D4-EDA4-4569-BC21-A23BC8EBAF80}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId19"/>
+  <drawing r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -27110,8 +27202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -27124,179 +27216,179 @@
   <sheetData>
     <row r="1" spans="1:4" ht="47.25" customHeight="1">
       <c r="A1" s="71" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B1" s="71"/>
     </row>
     <row r="2" spans="1:4" ht="72.75" customHeight="1">
       <c r="A2" s="73" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B2" s="74"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="72" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B3" s="72"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="183">
       <c r="A5" s="4" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="210">
       <c r="A6" s="4" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="210">
       <c r="A7" s="4" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="150">
       <c r="A8" s="4" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="255">
       <c r="A9" s="4" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="255">
       <c r="A10" s="4" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="315">
       <c r="A11" s="4" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="285">
       <c r="A12" s="4" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="255">
       <c r="A13" s="4" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="165">
       <c r="A14" s="4" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="165">
       <c r="A15" s="4" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="165">
       <c r="A16" s="4" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="225">
       <c r="A17" s="4" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="180">
       <c r="A18" s="4" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="105">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="106.5">
       <c r="A19" s="4" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="120">
       <c r="A20" s="4" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="135">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="137.25">
       <c r="A21" s="4" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -27330,82 +27422,82 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="28" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="26" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="25" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="26" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="26" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="F3" s="26"/>
       <c r="G3" s="31"/>
     </row>
     <row r="4" spans="1:7" ht="45">
       <c r="A4" s="26" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="29" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="36"/>
@@ -27415,10 +27507,10 @@
     </row>
     <row r="6" spans="1:7" ht="30">
       <c r="A6" s="29" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="36"/>
@@ -27428,10 +27520,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="29" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -27441,13 +27533,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="29" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
@@ -27456,13 +27548,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="29" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
@@ -27471,28 +27563,28 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="29" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="B10" s="37" t="str">
         <f xml:space="preserve"> HYPERLINK("#'Bibliography'!" &amp; ADDRESS(MATCH("Integrating Cybernetic Big Five Theory with the free energy Principle: A new strategy for modeling Personalities as complex systems", Bibliography!F:F, 0), 1), "CB5T+Free Energy Principle")</f>
         <v>CB5T+Free Energy Principle</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="29" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="29" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
@@ -27502,34 +27594,34 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="41" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="B12" s="27" t="str">
         <f xml:space="preserve"> HYPERLINK("#'Bibliography'!" &amp; ADDRESS(MATCH("Self-Entropic Broadening Theory: Toward a New Understanding of Self and Behavior Change Informed by Psychedelics and Psychosis", Bibliography!F:F, 0), 1), "SEBT Theory")</f>
         <v>SEBT Theory</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="26" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="31"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="41" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
@@ -27537,10 +27629,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="32" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="32"/>
@@ -27605,10 +27697,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="300">
@@ -27618,12 +27710,12 @@
     </row>
     <row r="3" spans="1:2" ht="270">
       <c r="B3" s="49" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="270">
       <c r="B4" s="49" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="300">
@@ -27633,37 +27725,37 @@
     </row>
     <row r="6" spans="1:2" ht="285">
       <c r="B6" s="45" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="285">
       <c r="B7" s="49" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="300">
       <c r="B8" s="49" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="240">
       <c r="B9" s="49" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="270">
       <c r="B10" s="49" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="345">
       <c r="B11" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="120">
       <c r="B12" s="49" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -27694,54 +27786,54 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="B1" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="75">
       <c r="A2" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="345">
       <c r="A3" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30">
       <c r="A4" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="225">
       <c r="A5" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" ht="210">
       <c r="A6" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="C6" t="e" vm="2">
         <v>#VALUE!</v>
@@ -27749,13 +27841,13 @@
     </row>
     <row r="7" spans="1:4" ht="300">
       <c r="A7" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified background for better contrast
</commit_message>
<xml_diff>
--- a/Excel_References.xlsx
+++ b/Excel_References.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/ennowinkler_ennosgermancourse_onmicrosoft_com/Documents/PhDProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1097" documentId="13_ncr:1_{92D5FB84-227A-4306-9187-93183921DEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC8C99B5-3A4A-43D4-861C-F9850FA32004}"/>
+  <xr:revisionPtr revIDLastSave="1106" documentId="13_ncr:1_{92D5FB84-227A-4306-9187-93183921DEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEC0F3FE-D4D4-4060-B41E-39608A23E3A1}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5460" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Notebook" sheetId="34" r:id="rId5"/>
     <sheet name="Stipendium" sheetId="35" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028" iterate="1" calcCompleted="0"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="271">
   <si>
     <t xml:space="preserve">@INCOLLECTION{Mauss2009-uk,   title = {Culture and automatic emotion regulation},   booktitle = {Regulating Emotions},   author = {Mauss, Iris B and Bunge, Silvia A and Gross, James J},   publisher = {Blackwell Publishing Ltd.},   pages = {39--60},   year = 2009,   address = {Oxford, UK} }  </t>
   </si>
@@ -1057,17 +1057,6 @@
   year = {2023},
   month = apr,
   pages = {886–893}
-}</t>
-  </si>
-  <si>
-    <t>@misc{Tracy2007,
-  title = {Authentic And Hubristic Pride Scales},
-  url = {http://dx.doi.org/10.1037/t06465-000},
-  DOI = {10.1037/t06465-000},
-  journal = {PsycTESTS Dataset},
-  publisher = {American Psychological Association (APA)},
-  author = {Tracy,  Jessica L. and Robins,  Richard W.},
-  year = {2007}
 }</t>
   </si>
   <si>
@@ -2261,6 +2250,28 @@
     <t>Kann ich mich ausschließlich für eine Förderung für einen Studien- oder Forschungsaufenthalt im Ausland bewerben, selbst wenn ich noch nicht Stipendiat*in bin?
 Studierende und Graduierte, die einen Auslandsaufenthalt planen, aber noch kein*e Stipendiat*innen der Heinrich-Böll-Stiftung sind, können nicht separat für einen Auslandsaufenthalt gefördert werden.</t>
   </si>
+  <si>
+    <t>@article{Tracy2007,
+  title = {Authentic And Hubristic Pride Scales},
+  url = {http://dx.doi.org/10.1037/t06465-000},
+  DOI = {10.1037/t06465-000},
+  journal = {PsycTESTS Dataset},
+  publisher = {American Psychological Association (APA)},
+  author = {Tracy,  Jessica L. and Robins,  Richard W.},
+  year = {2007}
+}</t>
+  </si>
+  <si>
+    <t>@manual{winter1994manual,
+  title     = {Manual for scoring motive imagery in running text},
+  author    = {Winter, David G.},
+  year      = {1994},
+  edition   = {4th},
+  note      = {Unpublished manuscript},
+  address   = {Ann Arbor},
+  institution = {University of Michigan},
+}</t>
+  </si>
 </sst>
 </file>
 
@@ -2709,9 +2720,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
-    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -2743,6 +2754,12 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color rgb="FF8EA9DB"/>
+        </left>
+        <top style="thin">
+          <color rgb="FF8EA9DB"/>
+        </top>
         <bottom style="thin">
           <color rgb="FF8EA9DB"/>
         </bottom>
@@ -2750,12 +2767,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF8EA9DB"/>
-        </left>
-        <top style="thin">
-          <color rgb="FF8EA9DB"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF8EA9DB"/>
         </bottom>
@@ -2861,7 +2872,7 @@
       <xdr:col>21</xdr:col>
       <xdr:colOff>398181</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>1449278</xdr:rowOff>
+      <xdr:rowOff>1449279</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3018,6 +3029,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
 <rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <global>
@@ -3088,7 +3103,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEE9F52D-586D-4F2A-94A6-4C9D6411A1D5}" name="Tabelle1" displayName="Tabelle1" ref="A1:G14" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEE9F52D-586D-4F2A-94A6-4C9D6411A1D5}" name="Tabelle1" displayName="Tabelle1" ref="A1:G14" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A1:G14" xr:uid="{DEE9F52D-586D-4F2A-94A6-4C9D6411A1D5}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3112,9 +3127,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3152,7 +3167,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3258,7 +3273,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3400,7 +3415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -19680,10 +19695,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S508"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="26.25"/>
@@ -19881,7 +19896,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="19"/>
     </row>
-    <row r="5" spans="1:19" ht="33.75">
+    <row r="5" spans="1:19" ht="52.5">
       <c r="A5" s="53" t="s">
         <v>33</v>
       </c>
@@ -19917,7 +19932,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="19"/>
     </row>
-    <row r="6" spans="1:19" ht="105">
+    <row r="6" spans="1:19" ht="90">
       <c r="A6" s="53" t="s">
         <v>34</v>
       </c>
@@ -20029,7 +20044,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="19"/>
     </row>
-    <row r="9" spans="1:19" ht="105">
+    <row r="9" spans="1:19" ht="90">
       <c r="A9" s="53" t="s">
         <v>39</v>
       </c>
@@ -20102,7 +20117,7 @@
       </c>
       <c r="H10" s="67">
         <f t="shared" ca="1" si="6"/>
-        <v>45439.816029745372</v>
+        <v>45535.740519212966</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>44</v>
@@ -20110,7 +20125,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="19"/>
     </row>
-    <row r="11" spans="1:19" ht="105">
+    <row r="11" spans="1:19" ht="90">
       <c r="A11" s="53" t="s">
         <v>45</v>
       </c>
@@ -20372,7 +20387,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="105">
+    <row r="17" spans="1:19" ht="90">
       <c r="A17" s="53" t="s">
         <v>66</v>
       </c>
@@ -20489,7 +20504,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="105">
+    <row r="20" spans="1:19" ht="90">
       <c r="A20" s="53" t="s">
         <v>71</v>
       </c>
@@ -21646,9 +21661,9 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" ht="33.75">
-      <c r="A50" s="53" t="s">
-        <v>125</v>
+    <row r="50" spans="1:11" ht="135">
+      <c r="A50" s="49" t="s">
+        <v>269</v>
       </c>
       <c r="B50" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21684,7 +21699,7 @@
     </row>
     <row r="51" spans="1:11" ht="78.75">
       <c r="A51" s="53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B51" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21720,7 +21735,7 @@
     </row>
     <row r="52" spans="1:11" ht="52.5">
       <c r="A52" s="53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B52" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21754,9 +21769,9 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" ht="121.5">
+    <row r="53" spans="1:11" ht="105">
       <c r="A53" s="54" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B53" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21787,16 +21802,16 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J53" s="1"/>
       <c r="K53" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="52.5">
       <c r="A54" s="54" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B54" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21827,14 +21842,14 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
     <row r="55" spans="1:11" ht="52.5">
       <c r="A55" s="54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B55" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21865,14 +21880,14 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
     <row r="56" spans="1:11" ht="63">
       <c r="A56" s="55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B56" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21903,14 +21918,14 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
     <row r="57" spans="1:11" ht="52.5">
       <c r="A57" s="54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B57" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21941,14 +21956,14 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
     <row r="58" spans="1:11" ht="63">
       <c r="A58" s="54" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B58" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21979,14 +21994,14 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
     <row r="59" spans="1:11" ht="42">
       <c r="A59" s="54" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B59" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22017,14 +22032,14 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
     <row r="60" spans="1:11" ht="52.5">
       <c r="A60" s="54" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B60" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22055,14 +22070,14 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
     <row r="61" spans="1:11" ht="33.75">
       <c r="A61" s="56" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B61" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22093,13 +22108,13 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J61" s="1"/>
     </row>
     <row r="62" spans="1:11" ht="52.5">
       <c r="A62" s="54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B62" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22134,7 +22149,7 @@
     </row>
     <row r="63" spans="1:11" ht="52.5">
       <c r="A63" s="53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B63" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22169,7 +22184,7 @@
     </row>
     <row r="64" spans="1:11" ht="33.75">
       <c r="A64" s="53" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B64" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22204,7 +22219,7 @@
     </row>
     <row r="65" spans="1:11" ht="52.5">
       <c r="A65" s="53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B65" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22239,7 +22254,7 @@
     </row>
     <row r="66" spans="1:11" ht="52.5">
       <c r="A66" s="53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B66" s="62" t="str">
         <f t="shared" ref="B66" si="15">IFERROR("@" &amp; MID(A66, SEARCH("{", A66) + 1, SEARCH(",", A66) - SEARCH("{", A66) - 1), "")</f>
@@ -22274,7 +22289,7 @@
     </row>
     <row r="67" spans="1:11" ht="52.5">
       <c r="A67" s="53" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B67" s="62" t="str">
         <f t="shared" ref="B67" si="22">IFERROR("@" &amp; MID(A67, SEARCH("{", A67) + 1, SEARCH(",", A67) - SEARCH("{", A67) - 1), "")</f>
@@ -22310,7 +22325,7 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B68" s="62" t="str">
         <f t="shared" ref="B68:B69" si="29">IFERROR("@" &amp; MID(A68, SEARCH("{", A68) + 1, SEARCH(",", A68) - SEARCH("{", A68) - 1), "")</f>
@@ -22344,7 +22359,7 @@
     </row>
     <row r="69" spans="1:11" ht="52.5">
       <c r="A69" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B69" s="62" t="str">
         <f t="shared" si="29"/>
@@ -22378,7 +22393,7 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B70" s="62" t="str">
         <f t="shared" ref="B70" si="36">IFERROR("@" &amp; MID(A70, SEARCH("{", A70) + 1, SEARCH(",", A70) - SEARCH("{", A70) - 1), "")</f>
@@ -22409,13 +22424,13 @@
         <v>45458.517281365741</v>
       </c>
       <c r="I70" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K70"/>
     </row>
     <row r="71" spans="1:11" ht="52.5">
       <c r="A71" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B71" s="62" t="str">
         <f t="shared" ref="B71" si="43">IFERROR("@" &amp; MID(A71, SEARCH("{", A71) + 1, SEARCH(",", A71) - SEARCH("{", A71) - 1), "")</f>
@@ -22446,13 +22461,13 @@
         <v>45458.535618402777</v>
       </c>
       <c r="I71" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K71"/>
     </row>
     <row r="72" spans="1:11" ht="63">
       <c r="A72" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B72" s="62" t="str">
         <f t="shared" ref="B72" si="50">IFERROR("@" &amp; MID(A72, SEARCH("{", A72) + 1, SEARCH(",", A72) - SEARCH("{", A72) - 1), "")</f>
@@ -22488,35 +22503,35 @@
         <v>35</v>
       </c>
       <c r="K72" s="42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B73" s="62" t="str">
-        <f t="shared" ref="B73:B83" si="57">IFERROR("@" &amp; MID(A73, SEARCH("{", A73) + 1, SEARCH(",", A73) - SEARCH("{", A73) - 1), "")</f>
+        <f t="shared" ref="B73:B84" si="57">IFERROR("@" &amp; MID(A73, SEARCH("{", A73) + 1, SEARCH(",", A73) - SEARCH("{", A73) - 1), "")</f>
         <v>@KeltnerMonroy2023</v>
       </c>
       <c r="C73" s="63" t="str">
-        <f t="shared" ref="C73:C83" si="58">"[" &amp; B73 &amp; "]"</f>
+        <f t="shared" ref="C73:C84" si="58">"[" &amp; B73 &amp; "]"</f>
         <v>[@KeltnerMonroy2023]</v>
       </c>
       <c r="D73" s="63" t="str">
-        <f t="shared" ref="D73:D83" si="59">IFERROR(MID(A73,SEARCH("year = {",A73)+8,4), "")</f>
+        <f t="shared" ref="D73:D84" si="59">IFERROR(MID(A73,SEARCH("year = {",A73)+8,4), "")</f>
         <v>2023</v>
       </c>
       <c r="E73" s="64" t="str">
-        <f t="shared" ref="E73:E83" si="60">IFERROR(MID(A73, SEARCH("author = {", A73) + 10, SEARCH("}", A73, SEARCH("author = {", A73)) - SEARCH("author = {", A73) - 10), "")</f>
+        <f t="shared" ref="E73:E84" si="60">IFERROR(MID(A73, SEARCH("author = {", A73) + 10, SEARCH("}", A73, SEARCH("author = {", A73)) - SEARCH("author = {", A73) - 10), "")</f>
         <v>Monroy, Maria and Keltner, Dacher</v>
       </c>
       <c r="F73" s="65" t="str">
-        <f t="shared" ref="F73:F83" si="61">IFERROR(IF(ISERROR(FIND("title =",A73)),"",MID(A73,FIND("title =",A73)+9,FIND("},",A73,FIND("title =",A73))-FIND("title =",A73)-9)),"")</f>
+        <f t="shared" ref="F73:F84" si="61">IFERROR(IF(ISERROR(FIND("title =",A73)),"",MID(A73,FIND("title =",A73)+9,FIND("},",A73,FIND("title =",A73))-FIND("title =",A73)-9)),"")</f>
         <v>Awe as a Pathway to Mental and Physical Health</v>
       </c>
       <c r="G73" s="66" t="str">
-        <f t="shared" ref="G73:G83" si="62">IFERROR("https://doi.org/" &amp; MID(A73, SEARCH("doi = {", A73) + 7, FIND("}", A73, SEARCH("doi = {", A73)) - SEARCH("doi = {", A73) - 7),"")</f>
+        <f t="shared" ref="G73:G84" si="62">IFERROR("https://doi.org/" &amp; MID(A73, SEARCH("doi = {", A73) + 7, FIND("}", A73, SEARCH("doi = {", A73)) - SEARCH("doi = {", A73) - 7),"")</f>
         <v>https://doi.org/10.1177/17456916221094856</v>
       </c>
       <c r="H73" s="67">
@@ -22524,13 +22539,13 @@
         <v>45526.456741666669</v>
       </c>
       <c r="I73" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K73"/>
     </row>
     <row r="74" spans="1:11" ht="180">
       <c r="A74" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B74" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22561,13 +22576,13 @@
         <v>45526.459042361108</v>
       </c>
       <c r="I74" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K74"/>
     </row>
     <row r="75" spans="1:11" ht="195">
       <c r="A75" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B75" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22601,7 +22616,7 @@
     </row>
     <row r="76" spans="1:11" ht="345">
       <c r="A76" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B76" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22638,7 +22653,7 @@
     </row>
     <row r="77" spans="1:11" ht="240">
       <c r="A77" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B77" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22672,7 +22687,7 @@
     </row>
     <row r="78" spans="1:11" ht="240">
       <c r="A78" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B78" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22704,9 +22719,9 @@
       </c>
       <c r="K78"/>
     </row>
-    <row r="79" spans="1:11" ht="152.25">
+    <row r="79" spans="1:11" ht="150">
       <c r="A79" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B79" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22739,9 +22754,9 @@
       </c>
       <c r="K79"/>
     </row>
-    <row r="80" spans="1:11" ht="244.5">
+    <row r="80" spans="1:11" ht="240">
       <c r="A80" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B80" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22773,9 +22788,9 @@
       </c>
       <c r="K80"/>
     </row>
-    <row r="81" spans="1:18" ht="121.5">
+    <row r="81" spans="1:18" ht="120">
       <c r="A81" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B81" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22812,12 +22827,12 @@
         <v>58</v>
       </c>
       <c r="K81" s="42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" ht="165">
+      <c r="A82" s="4" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18" ht="167.25">
-      <c r="A82" s="4" t="s">
-        <v>164</v>
       </c>
       <c r="B82" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22851,15 +22866,15 @@
         <v>58</v>
       </c>
       <c r="K82" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="R82" t="s">
         <v>165</v>
       </c>
-      <c r="R82" t="s">
+    </row>
+    <row r="83" spans="1:18" ht="105">
+      <c r="A83" s="4" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="83" spans="1:18" ht="91.5">
-      <c r="A83" s="4" t="s">
-        <v>167</v>
       </c>
       <c r="B83" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22891,14 +22906,38 @@
       </c>
       <c r="K83"/>
     </row>
-    <row r="84" spans="1:18" ht="15">
-      <c r="B84" s="68"/>
-      <c r="C84" s="68"/>
-      <c r="D84" s="68"/>
-      <c r="E84" s="69"/>
-      <c r="F84" s="68"/>
-      <c r="G84" s="68"/>
-      <c r="H84" s="68"/>
+    <row r="84" spans="1:18" ht="135">
+      <c r="A84" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B84" s="62" t="str">
+        <f t="shared" ref="B84" si="64">IFERROR("@" &amp; MID(A84, SEARCH("{", A84) + 1, SEARCH(",", A84) - SEARCH("{", A84) - 1), "")</f>
+        <v>@winter1994manual</v>
+      </c>
+      <c r="C84" s="63" t="str">
+        <f t="shared" ref="C84" si="65">"[" &amp; B84 &amp; "]"</f>
+        <v>[@winter1994manual]</v>
+      </c>
+      <c r="D84" s="63" t="str">
+        <f t="shared" ref="D84" si="66">IFERROR(MID(A84,SEARCH("year = {",A84)+8,4), "")</f>
+        <v/>
+      </c>
+      <c r="E84" s="64" t="str">
+        <f t="shared" ref="E84" si="67">IFERROR(MID(A84, SEARCH("author = {", A84) + 10, SEARCH("}", A84, SEARCH("author = {", A84)) - SEARCH("author = {", A84) - 10), "")</f>
+        <v/>
+      </c>
+      <c r="F84" s="65" t="str">
+        <f t="shared" ref="F84" si="68">IFERROR(IF(ISERROR(FIND("title =",A84)),"",MID(A84,FIND("title =",A84)+9,FIND("},",A84,FIND("title =",A84))-FIND("title =",A84)-9)),"")</f>
+        <v/>
+      </c>
+      <c r="G84" s="66" t="str">
+        <f t="shared" ref="G84" si="69">IFERROR("https://doi.org/" &amp; MID(A84, SEARCH("doi = {", A84) + 7, FIND("}", A84, SEARCH("doi = {", A84)) - SEARCH("doi = {", A84) - 7),"")</f>
+        <v/>
+      </c>
+      <c r="H84" s="67">
+        <f t="shared" ref="H84" ca="1" si="70">IF(A84&lt;&gt;"",IF(H84&lt;&gt;"",H84,NOW()),"")</f>
+        <v>45528.541320486111</v>
+      </c>
       <c r="K84"/>
     </row>
     <row r="85" spans="1:18" ht="15">
@@ -27149,7 +27188,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S509">
     <sortCondition ref="H1:H509"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D83">
+  <conditionalFormatting sqref="D2:D84">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -27159,7 +27198,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D509:D1048576 D1:D83">
+  <conditionalFormatting sqref="D509:D1048576 D1:D84">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -27216,179 +27255,179 @@
   <sheetData>
     <row r="1" spans="1:4" ht="47.25" customHeight="1">
       <c r="A1" s="71" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B1" s="71"/>
     </row>
     <row r="2" spans="1:4" ht="72.75" customHeight="1">
       <c r="A2" s="73" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" s="74"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="72" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" s="72"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="180">
+      <c r="A5" s="4" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="183">
-      <c r="A5" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="210">
       <c r="A6" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="210">
       <c r="A7" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="150">
       <c r="A8" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="255">
       <c r="A9" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="255">
       <c r="A10" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="315">
       <c r="A11" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="285">
       <c r="A12" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="255">
       <c r="A13" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="165">
       <c r="A14" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="165">
       <c r="A15" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="165">
       <c r="A16" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="225">
       <c r="A17" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="180">
       <c r="A18" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B18" s="4" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="105">
+      <c r="A19" s="4" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="106.5">
-      <c r="A19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="120">
       <c r="A20" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B20" s="4" t="s">
+    </row>
+    <row r="21" spans="1:3" ht="135">
+      <c r="A21" s="4" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="137.25">
-      <c r="A21" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -27422,82 +27461,82 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="C1" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="D1" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="E1" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="F1" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="G1" s="24" t="s">
         <v>217</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="26" t="s">
         <v>220</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>221</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="C3" s="16" t="s">
         <v>224</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>225</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F3" s="26"/>
       <c r="G3" s="31"/>
     </row>
     <row r="4" spans="1:7" ht="45">
       <c r="A4" s="26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="35" t="s">
         <v>229</v>
-      </c>
-      <c r="B5" s="35" t="s">
-        <v>230</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="36"/>
@@ -27507,10 +27546,10 @@
     </row>
     <row r="6" spans="1:7" ht="30">
       <c r="A6" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" s="35" t="s">
         <v>231</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>232</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="36"/>
@@ -27520,10 +27559,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="B7" s="38" t="s">
         <v>233</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>234</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -27533,13 +27572,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="B8" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="C8" s="29" t="s">
         <v>236</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>237</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
@@ -27548,13 +27587,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="B9" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="C9" s="29" t="s">
         <v>239</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>240</v>
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
@@ -27563,28 +27602,28 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="29" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B10" s="37" t="str">
         <f xml:space="preserve"> HYPERLINK("#'Bibliography'!" &amp; ADDRESS(MATCH("Integrating Cybernetic Big Five Theory with the free energy Principle: A new strategy for modeling Personalities as complex systems", Bibliography!F:F, 0), 1), "CB5T+Free Energy Principle")</f>
         <v>CB5T+Free Energy Principle</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="29" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
@@ -27594,34 +27633,34 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="41" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B12" s="27" t="str">
         <f xml:space="preserve"> HYPERLINK("#'Bibliography'!" &amp; ADDRESS(MATCH("Self-Entropic Broadening Theory: Toward a New Understanding of Self and Behavior Change Informed by Psychedelics and Psychosis", Bibliography!F:F, 0), 1), "SEBT Theory")</f>
         <v>SEBT Theory</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="31"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="B13" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="C13" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="D13" s="25" t="s">
         <v>247</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>248</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
@@ -27629,10 +27668,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="B14" s="40" t="s">
         <v>249</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>250</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="32"/>
@@ -27697,25 +27736,25 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="42" t="s">
         <v>251</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="300">
       <c r="B2" s="49" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="270">
       <c r="B3" s="49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="270">
       <c r="B4" s="49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="300">
@@ -27725,37 +27764,37 @@
     </row>
     <row r="6" spans="1:2" ht="285">
       <c r="B6" s="45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="285">
       <c r="B7" s="49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="300">
       <c r="B8" s="49" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="240">
       <c r="B9" s="49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="270">
       <c r="B10" s="49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="345">
       <c r="B11" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="120">
       <c r="B12" s="49" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -27786,54 +27825,54 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B1" t="s">
         <v>254</v>
-      </c>
-      <c r="B1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="75">
       <c r="A2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>256</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="345">
       <c r="A3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" s="47" t="s">
         <v>258</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30">
       <c r="A4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B4" s="46" t="s">
         <v>260</v>
-      </c>
-      <c r="B4" s="46" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="225">
       <c r="A5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B5" s="48" t="s">
         <v>262</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="C5" s="8" t="s">
         <v>263</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>264</v>
       </c>
       <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" ht="210">
       <c r="A6" t="s">
+        <v>264</v>
+      </c>
+      <c r="B6" s="46" t="s">
         <v>265</v>
-      </c>
-      <c r="B6" s="46" t="s">
-        <v>266</v>
       </c>
       <c r="C6" t="e" vm="2">
         <v>#VALUE!</v>
@@ -27841,13 +27880,13 @@
     </row>
     <row r="7" spans="1:4" ht="300">
       <c r="A7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B7" s="46" t="s">
         <v>267</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="C7" s="46" t="s">
         <v>268</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I think this is now a good draft that will just need minor adjustments
</commit_message>
<xml_diff>
--- a/Excel_References.xlsx
+++ b/Excel_References.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/ennowinkler_ennosgermancourse_onmicrosoft_com/Documents/PhDProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1106" documentId="13_ncr:1_{92D5FB84-227A-4306-9187-93183921DEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEC0F3FE-D4D4-4060-B41E-39608A23E3A1}"/>
+  <xr:revisionPtr revIDLastSave="1110" documentId="13_ncr:1_{92D5FB84-227A-4306-9187-93183921DEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{488E90A1-5B66-4112-9B59-8FFB30581770}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5460" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Notebook" sheetId="34" r:id="rId5"/>
     <sheet name="Stipendium" sheetId="35" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191028" iterate="1" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="272">
   <si>
     <t xml:space="preserve">@INCOLLECTION{Mauss2009-uk,   title = {Culture and automatic emotion regulation},   booktitle = {Regulating Emotions},   author = {Mauss, Iris B and Bunge, Silvia A and Gross, James J},   publisher = {Blackwell Publishing Ltd.},   pages = {39--60},   year = 2009,   address = {Oxford, UK} }  </t>
   </si>
@@ -1060,6 +1060,17 @@
 }</t>
   </si>
   <si>
+    <t>@article{Tracy2007,
+  title = {Authentic And Hubristic Pride Scales},
+  url = {http://dx.doi.org/10.1037/t06465-000},
+  DOI = {10.1037/t06465-000},
+  journal = {PsycTESTS Dataset},
+  publisher = {American Psychological Association (APA)},
+  author = {Tracy,  Jessica L. and Robins,  Richard W.},
+  year = {2007}
+}</t>
+  </si>
+  <si>
     <t>@article{Schultheiss2008,
   title = {The reliability of a Picture Story Exercise measure of implicit motives: Estimates of internal consistency,  retest reliability,  and ipsative stability},
   volume = {42},
@@ -1592,6 +1603,33 @@
   author = {Tiberius, Valerie},
   year = {2018},
   publisher = {Oxford University Press, USA}
+}</t>
+  </si>
+  <si>
+    <t>@manual{winter1994manual,
+  title     = {Manual for scoring motive imagery in running text},
+  author    = {Winter, David G.},
+  year      = {1994},
+  edition   = {4th},
+  note      = {Unpublished manuscript},
+  address   = {Ann Arbor},
+  institution = {University of Michigan},
+}</t>
+  </si>
+  <si>
+    <t>@article{Dong2019,
+  title = {Openness to Experience,  Extraversion,  and Subjective Well-Being Among Chinese College Students: The Mediating Role of Dispositional Awe},
+  volume = {123},
+  ISSN = {1558-691X},
+  url = {http://dx.doi.org/10.1177/0033294119826884},
+  DOI = {10.1177/0033294119826884},
+  number = {3},
+  journal = {Psychological Reports},
+  publisher = {SAGE Publications},
+  author = {Dong,  Rui and Ni,  Shi G.},
+  year = {2019},
+  month = feb,
+  pages = {903–928}
 }</t>
   </si>
   <si>
@@ -2250,28 +2288,6 @@
     <t>Kann ich mich ausschließlich für eine Förderung für einen Studien- oder Forschungsaufenthalt im Ausland bewerben, selbst wenn ich noch nicht Stipendiat*in bin?
 Studierende und Graduierte, die einen Auslandsaufenthalt planen, aber noch kein*e Stipendiat*innen der Heinrich-Böll-Stiftung sind, können nicht separat für einen Auslandsaufenthalt gefördert werden.</t>
   </si>
-  <si>
-    <t>@article{Tracy2007,
-  title = {Authentic And Hubristic Pride Scales},
-  url = {http://dx.doi.org/10.1037/t06465-000},
-  DOI = {10.1037/t06465-000},
-  journal = {PsycTESTS Dataset},
-  publisher = {American Psychological Association (APA)},
-  author = {Tracy,  Jessica L. and Robins,  Richard W.},
-  year = {2007}
-}</t>
-  </si>
-  <si>
-    <t>@manual{winter1994manual,
-  title     = {Manual for scoring motive imagery in running text},
-  author    = {Winter, David G.},
-  year      = {1994},
-  edition   = {4th},
-  note      = {Unpublished manuscript},
-  address   = {Ann Arbor},
-  institution = {University of Michigan},
-}</t>
-  </si>
 </sst>
 </file>
 
@@ -2720,9 +2736,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -2754,12 +2770,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF8EA9DB"/>
-        </left>
-        <top style="thin">
-          <color rgb="FF8EA9DB"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF8EA9DB"/>
         </bottom>
@@ -2767,6 +2777,12 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color rgb="FF8EA9DB"/>
+        </left>
+        <top style="thin">
+          <color rgb="FF8EA9DB"/>
+        </top>
         <bottom style="thin">
           <color rgb="FF8EA9DB"/>
         </bottom>
@@ -3029,10 +3045,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
 <rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <global>
@@ -3103,7 +3115,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEE9F52D-586D-4F2A-94A6-4C9D6411A1D5}" name="Tabelle1" displayName="Tabelle1" ref="A1:G14" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEE9F52D-586D-4F2A-94A6-4C9D6411A1D5}" name="Tabelle1" displayName="Tabelle1" ref="A1:G14" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8">
   <autoFilter ref="A1:G14" xr:uid="{DEE9F52D-586D-4F2A-94A6-4C9D6411A1D5}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3127,9 +3139,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3167,7 +3179,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3273,7 +3285,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3415,7 +3427,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -19696,9 +19708,9 @@
   <dimension ref="A1:S508"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
       <selection activeCell="B5" sqref="B5"/>
-      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="26.25"/>
@@ -21663,7 +21675,7 @@
     </row>
     <row r="50" spans="1:11" ht="135">
       <c r="A50" s="49" t="s">
-        <v>269</v>
+        <v>125</v>
       </c>
       <c r="B50" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21699,7 +21711,7 @@
     </row>
     <row r="51" spans="1:11" ht="78.75">
       <c r="A51" s="53" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B51" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21735,7 +21747,7 @@
     </row>
     <row r="52" spans="1:11" ht="52.5">
       <c r="A52" s="53" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B52" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21771,7 +21783,7 @@
     </row>
     <row r="53" spans="1:11" ht="105">
       <c r="A53" s="54" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B53" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21802,16 +21814,16 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J53" s="1"/>
       <c r="K53" s="43" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="52.5">
       <c r="A54" s="54" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B54" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21842,14 +21854,14 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
     <row r="55" spans="1:11" ht="52.5">
       <c r="A55" s="54" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B55" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21880,14 +21892,14 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
     <row r="56" spans="1:11" ht="63">
       <c r="A56" s="55" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B56" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21918,14 +21930,14 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
     <row r="57" spans="1:11" ht="52.5">
       <c r="A57" s="54" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B57" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21956,14 +21968,14 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
     <row r="58" spans="1:11" ht="63">
       <c r="A58" s="54" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B58" s="62" t="str">
         <f t="shared" si="9"/>
@@ -21994,14 +22006,14 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
     <row r="59" spans="1:11" ht="42">
       <c r="A59" s="54" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B59" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22032,14 +22044,14 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
     <row r="60" spans="1:11" ht="52.5">
       <c r="A60" s="54" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B60" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22070,14 +22082,14 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
     <row r="61" spans="1:11" ht="33.75">
       <c r="A61" s="56" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B61" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22108,13 +22120,13 @@
         <v>45450.905073148147</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J61" s="1"/>
     </row>
     <row r="62" spans="1:11" ht="52.5">
       <c r="A62" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B62" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22149,7 +22161,7 @@
     </row>
     <row r="63" spans="1:11" ht="52.5">
       <c r="A63" s="53" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B63" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22184,7 +22196,7 @@
     </row>
     <row r="64" spans="1:11" ht="33.75">
       <c r="A64" s="53" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B64" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22219,7 +22231,7 @@
     </row>
     <row r="65" spans="1:11" ht="52.5">
       <c r="A65" s="53" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B65" s="62" t="str">
         <f t="shared" si="9"/>
@@ -22254,7 +22266,7 @@
     </row>
     <row r="66" spans="1:11" ht="52.5">
       <c r="A66" s="53" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B66" s="62" t="str">
         <f t="shared" ref="B66" si="15">IFERROR("@" &amp; MID(A66, SEARCH("{", A66) + 1, SEARCH(",", A66) - SEARCH("{", A66) - 1), "")</f>
@@ -22289,7 +22301,7 @@
     </row>
     <row r="67" spans="1:11" ht="52.5">
       <c r="A67" s="53" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B67" s="62" t="str">
         <f t="shared" ref="B67" si="22">IFERROR("@" &amp; MID(A67, SEARCH("{", A67) + 1, SEARCH(",", A67) - SEARCH("{", A67) - 1), "")</f>
@@ -22325,7 +22337,7 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B68" s="62" t="str">
         <f t="shared" ref="B68:B69" si="29">IFERROR("@" &amp; MID(A68, SEARCH("{", A68) + 1, SEARCH(",", A68) - SEARCH("{", A68) - 1), "")</f>
@@ -22359,7 +22371,7 @@
     </row>
     <row r="69" spans="1:11" ht="52.5">
       <c r="A69" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B69" s="62" t="str">
         <f t="shared" si="29"/>
@@ -22393,7 +22405,7 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B70" s="62" t="str">
         <f t="shared" ref="B70" si="36">IFERROR("@" &amp; MID(A70, SEARCH("{", A70) + 1, SEARCH(",", A70) - SEARCH("{", A70) - 1), "")</f>
@@ -22424,13 +22436,13 @@
         <v>45458.517281365741</v>
       </c>
       <c r="I70" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K70"/>
     </row>
     <row r="71" spans="1:11" ht="52.5">
       <c r="A71" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B71" s="62" t="str">
         <f t="shared" ref="B71" si="43">IFERROR("@" &amp; MID(A71, SEARCH("{", A71) + 1, SEARCH(",", A71) - SEARCH("{", A71) - 1), "")</f>
@@ -22461,13 +22473,13 @@
         <v>45458.535618402777</v>
       </c>
       <c r="I71" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K71"/>
     </row>
     <row r="72" spans="1:11" ht="63">
       <c r="A72" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B72" s="62" t="str">
         <f t="shared" ref="B72" si="50">IFERROR("@" &amp; MID(A72, SEARCH("{", A72) + 1, SEARCH(",", A72) - SEARCH("{", A72) - 1), "")</f>
@@ -22503,12 +22515,12 @@
         <v>35</v>
       </c>
       <c r="K72" s="42" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B73" s="62" t="str">
         <f t="shared" ref="B73:B84" si="57">IFERROR("@" &amp; MID(A73, SEARCH("{", A73) + 1, SEARCH(",", A73) - SEARCH("{", A73) - 1), "")</f>
@@ -22539,13 +22551,13 @@
         <v>45526.456741666669</v>
       </c>
       <c r="I73" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K73"/>
     </row>
     <row r="74" spans="1:11" ht="180">
       <c r="A74" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B74" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22576,13 +22588,13 @@
         <v>45526.459042361108</v>
       </c>
       <c r="I74" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K74"/>
     </row>
     <row r="75" spans="1:11" ht="195">
       <c r="A75" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B75" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22616,7 +22628,7 @@
     </row>
     <row r="76" spans="1:11" ht="345">
       <c r="A76" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B76" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22653,7 +22665,7 @@
     </row>
     <row r="77" spans="1:11" ht="240">
       <c r="A77" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B77" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22687,7 +22699,7 @@
     </row>
     <row r="78" spans="1:11" ht="240">
       <c r="A78" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B78" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22721,7 +22733,7 @@
     </row>
     <row r="79" spans="1:11" ht="150">
       <c r="A79" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B79" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22756,7 +22768,7 @@
     </row>
     <row r="80" spans="1:11" ht="240">
       <c r="A80" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B80" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22790,7 +22802,7 @@
     </row>
     <row r="81" spans="1:18" ht="120">
       <c r="A81" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B81" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22827,12 +22839,12 @@
         <v>58</v>
       </c>
       <c r="K81" s="42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="82" spans="1:18" ht="165">
       <c r="A82" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B82" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22866,15 +22878,15 @@
         <v>58</v>
       </c>
       <c r="K82" s="42" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="R82" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="1:18" ht="105">
       <c r="A83" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B83" s="62" t="str">
         <f t="shared" si="57"/>
@@ -22908,7 +22920,7 @@
     </row>
     <row r="84" spans="1:18" ht="135">
       <c r="A84" s="4" t="s">
-        <v>270</v>
+        <v>168</v>
       </c>
       <c r="B84" s="62" t="str">
         <f t="shared" ref="B84" si="64">IFERROR("@" &amp; MID(A84, SEARCH("{", A84) + 1, SEARCH(",", A84) - SEARCH("{", A84) - 1), "")</f>
@@ -22940,74 +22952,224 @@
       </c>
       <c r="K84"/>
     </row>
-    <row r="85" spans="1:18" ht="15">
-      <c r="B85" s="68"/>
-      <c r="C85" s="68"/>
-      <c r="D85" s="68"/>
-      <c r="E85" s="69"/>
-      <c r="F85" s="68"/>
-      <c r="G85" s="68"/>
-      <c r="H85" s="68"/>
+    <row r="85" spans="1:18" ht="229.5">
+      <c r="A85" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B85" s="62" t="str">
+        <f t="shared" ref="B85:B91" si="71">IFERROR("@" &amp; MID(A85, SEARCH("{", A85) + 1, SEARCH(",", A85) - SEARCH("{", A85) - 1), "")</f>
+        <v>@Dong2019</v>
+      </c>
+      <c r="C85" s="63" t="str">
+        <f t="shared" ref="C85:C91" si="72">"[" &amp; B85 &amp; "]"</f>
+        <v>[@Dong2019]</v>
+      </c>
+      <c r="D85" s="63" t="str">
+        <f t="shared" ref="D85:D91" si="73">IFERROR(MID(A85,SEARCH("year = {",A85)+8,4), "")</f>
+        <v>2019</v>
+      </c>
+      <c r="E85" s="64" t="str">
+        <f t="shared" ref="E85:E91" si="74">IFERROR(MID(A85, SEARCH("author = {", A85) + 10, SEARCH("}", A85, SEARCH("author = {", A85)) - SEARCH("author = {", A85) - 10), "")</f>
+        <v>Dong,  Rui and Ni,  Shi G.</v>
+      </c>
+      <c r="F85" s="65" t="str">
+        <f t="shared" ref="F85:F91" si="75">IFERROR(IF(ISERROR(FIND("title =",A85)),"",MID(A85,FIND("title =",A85)+9,FIND("},",A85,FIND("title =",A85))-FIND("title =",A85)-9)),"")</f>
+        <v>Openness to Experience,  Extraversion,  and Subjective Well-Being Among Chinese College Students: The Mediating Role of Dispositional Awe</v>
+      </c>
+      <c r="G85" s="66" t="str">
+        <f t="shared" ref="G85:G91" si="76">IFERROR("https://doi.org/" &amp; MID(A85, SEARCH("doi = {", A85) + 7, FIND("}", A85, SEARCH("doi = {", A85)) - SEARCH("doi = {", A85) - 7),"")</f>
+        <v>https://doi.org/10.1177/0033294119826884</v>
+      </c>
+      <c r="H85" s="67">
+        <f t="shared" ref="H85:H91" ca="1" si="77">IF(A85&lt;&gt;"",IF(H85&lt;&gt;"",H85,NOW()),"")</f>
+        <v>45537.942811805558</v>
+      </c>
       <c r="K85"/>
     </row>
-    <row r="86" spans="1:18" ht="15">
-      <c r="B86" s="68"/>
-      <c r="C86" s="68"/>
-      <c r="D86" s="68"/>
-      <c r="E86" s="69"/>
-      <c r="F86" s="68"/>
-      <c r="G86" s="68"/>
-      <c r="H86" s="68"/>
+    <row r="86" spans="1:18">
+      <c r="B86" s="62" t="str">
+        <f t="shared" si="71"/>
+        <v/>
+      </c>
+      <c r="C86" s="63" t="str">
+        <f t="shared" si="72"/>
+        <v>[]</v>
+      </c>
+      <c r="D86" s="63" t="str">
+        <f t="shared" si="73"/>
+        <v/>
+      </c>
+      <c r="E86" s="64" t="str">
+        <f t="shared" si="74"/>
+        <v/>
+      </c>
+      <c r="F86" s="65" t="str">
+        <f t="shared" si="75"/>
+        <v/>
+      </c>
+      <c r="G86" s="66" t="str">
+        <f t="shared" si="76"/>
+        <v/>
+      </c>
+      <c r="H86" s="67" t="str">
+        <f t="shared" ca="1" si="77"/>
+        <v/>
+      </c>
       <c r="K86"/>
     </row>
-    <row r="87" spans="1:18" ht="15">
-      <c r="B87" s="68"/>
-      <c r="C87" s="68"/>
-      <c r="D87" s="68"/>
-      <c r="E87" s="69"/>
-      <c r="F87" s="68"/>
-      <c r="G87" s="68"/>
-      <c r="H87" s="68"/>
+    <row r="87" spans="1:18">
+      <c r="B87" s="62" t="str">
+        <f t="shared" si="71"/>
+        <v/>
+      </c>
+      <c r="C87" s="63" t="str">
+        <f t="shared" si="72"/>
+        <v>[]</v>
+      </c>
+      <c r="D87" s="63" t="str">
+        <f t="shared" si="73"/>
+        <v/>
+      </c>
+      <c r="E87" s="64" t="str">
+        <f t="shared" si="74"/>
+        <v/>
+      </c>
+      <c r="F87" s="65" t="str">
+        <f t="shared" si="75"/>
+        <v/>
+      </c>
+      <c r="G87" s="66" t="str">
+        <f t="shared" si="76"/>
+        <v/>
+      </c>
+      <c r="H87" s="67" t="str">
+        <f t="shared" ca="1" si="77"/>
+        <v/>
+      </c>
       <c r="K87"/>
     </row>
-    <row r="88" spans="1:18" ht="15">
-      <c r="B88" s="68"/>
-      <c r="C88" s="68"/>
-      <c r="D88" s="68"/>
-      <c r="E88" s="69"/>
-      <c r="F88" s="68"/>
-      <c r="G88" s="68"/>
-      <c r="H88" s="68"/>
+    <row r="88" spans="1:18">
+      <c r="B88" s="62" t="str">
+        <f t="shared" si="71"/>
+        <v/>
+      </c>
+      <c r="C88" s="63" t="str">
+        <f t="shared" si="72"/>
+        <v>[]</v>
+      </c>
+      <c r="D88" s="63" t="str">
+        <f t="shared" si="73"/>
+        <v/>
+      </c>
+      <c r="E88" s="64" t="str">
+        <f t="shared" si="74"/>
+        <v/>
+      </c>
+      <c r="F88" s="65" t="str">
+        <f t="shared" si="75"/>
+        <v/>
+      </c>
+      <c r="G88" s="66" t="str">
+        <f t="shared" si="76"/>
+        <v/>
+      </c>
+      <c r="H88" s="67" t="str">
+        <f t="shared" ca="1" si="77"/>
+        <v/>
+      </c>
       <c r="K88"/>
     </row>
-    <row r="89" spans="1:18" ht="15">
-      <c r="B89" s="68"/>
-      <c r="C89" s="68"/>
-      <c r="D89" s="68"/>
-      <c r="E89" s="69"/>
-      <c r="F89" s="68"/>
-      <c r="G89" s="68"/>
-      <c r="H89" s="68"/>
+    <row r="89" spans="1:18">
+      <c r="B89" s="62" t="str">
+        <f t="shared" si="71"/>
+        <v/>
+      </c>
+      <c r="C89" s="63" t="str">
+        <f t="shared" si="72"/>
+        <v>[]</v>
+      </c>
+      <c r="D89" s="63" t="str">
+        <f t="shared" si="73"/>
+        <v/>
+      </c>
+      <c r="E89" s="64" t="str">
+        <f t="shared" si="74"/>
+        <v/>
+      </c>
+      <c r="F89" s="65" t="str">
+        <f t="shared" si="75"/>
+        <v/>
+      </c>
+      <c r="G89" s="66" t="str">
+        <f t="shared" si="76"/>
+        <v/>
+      </c>
+      <c r="H89" s="67" t="str">
+        <f t="shared" ca="1" si="77"/>
+        <v/>
+      </c>
       <c r="K89"/>
     </row>
-    <row r="90" spans="1:18" ht="15">
-      <c r="B90" s="68"/>
-      <c r="C90" s="68"/>
-      <c r="D90" s="68"/>
-      <c r="E90" s="69"/>
-      <c r="F90" s="68"/>
-      <c r="G90" s="68"/>
-      <c r="H90" s="68"/>
+    <row r="90" spans="1:18">
+      <c r="B90" s="62" t="str">
+        <f t="shared" si="71"/>
+        <v/>
+      </c>
+      <c r="C90" s="63" t="str">
+        <f t="shared" si="72"/>
+        <v>[]</v>
+      </c>
+      <c r="D90" s="63" t="str">
+        <f t="shared" si="73"/>
+        <v/>
+      </c>
+      <c r="E90" s="64" t="str">
+        <f t="shared" si="74"/>
+        <v/>
+      </c>
+      <c r="F90" s="65" t="str">
+        <f t="shared" si="75"/>
+        <v/>
+      </c>
+      <c r="G90" s="66" t="str">
+        <f t="shared" si="76"/>
+        <v/>
+      </c>
+      <c r="H90" s="67" t="str">
+        <f t="shared" ca="1" si="77"/>
+        <v/>
+      </c>
       <c r="K90"/>
     </row>
-    <row r="91" spans="1:18" ht="15">
-      <c r="B91" s="68"/>
-      <c r="C91" s="68"/>
-      <c r="D91" s="68"/>
-      <c r="E91" s="69"/>
-      <c r="F91" s="68"/>
-      <c r="G91" s="68"/>
-      <c r="H91" s="68"/>
+    <row r="91" spans="1:18">
+      <c r="B91" s="62" t="str">
+        <f t="shared" si="71"/>
+        <v/>
+      </c>
+      <c r="C91" s="63" t="str">
+        <f t="shared" si="72"/>
+        <v>[]</v>
+      </c>
+      <c r="D91" s="63" t="str">
+        <f t="shared" si="73"/>
+        <v/>
+      </c>
+      <c r="E91" s="64" t="str">
+        <f t="shared" si="74"/>
+        <v/>
+      </c>
+      <c r="F91" s="65" t="str">
+        <f t="shared" si="75"/>
+        <v/>
+      </c>
+      <c r="G91" s="66" t="str">
+        <f t="shared" si="76"/>
+        <v/>
+      </c>
+      <c r="H91" s="67" t="str">
+        <f t="shared" ca="1" si="77"/>
+        <v/>
+      </c>
       <c r="K91"/>
     </row>
     <row r="92" spans="1:18" ht="15">
@@ -27188,7 +27350,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S509">
     <sortCondition ref="H1:H509"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D84">
+  <conditionalFormatting sqref="D2:D91">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -27198,7 +27360,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D509:D1048576 D1:D84">
+  <conditionalFormatting sqref="D509:D1048576 D1:D91">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -27255,179 +27417,179 @@
   <sheetData>
     <row r="1" spans="1:4" ht="47.25" customHeight="1">
       <c r="A1" s="71" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B1" s="71"/>
     </row>
     <row r="2" spans="1:4" ht="72.75" customHeight="1">
       <c r="A2" s="73" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B2" s="74"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="72" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B3" s="72"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="180">
       <c r="A5" s="4" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="210">
       <c r="A6" s="4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="210">
       <c r="A7" s="4" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="150">
       <c r="A8" s="4" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="255">
       <c r="A9" s="4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="255">
       <c r="A10" s="4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="315">
       <c r="A11" s="4" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="285">
       <c r="A12" s="4" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="255">
       <c r="A13" s="4" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="165">
       <c r="A14" s="4" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="165">
       <c r="A15" s="4" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="165">
       <c r="A16" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="225">
       <c r="A17" s="4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="180">
       <c r="A18" s="4" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="105">
       <c r="A19" s="4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="120">
       <c r="A20" s="4" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="135">
       <c r="A21" s="4" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -27461,82 +27623,82 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="28" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="26" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="25" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="26" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="26" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="F3" s="26"/>
       <c r="G3" s="31"/>
     </row>
     <row r="4" spans="1:7" ht="45">
       <c r="A4" s="26" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="29" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="36"/>
@@ -27546,10 +27708,10 @@
     </row>
     <row r="6" spans="1:7" ht="30">
       <c r="A6" s="29" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="36"/>
@@ -27559,10 +27721,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="29" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -27572,13 +27734,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="29" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
@@ -27587,13 +27749,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="29" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
@@ -27602,28 +27764,28 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="29" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B10" s="37" t="str">
         <f xml:space="preserve"> HYPERLINK("#'Bibliography'!" &amp; ADDRESS(MATCH("Integrating Cybernetic Big Five Theory with the free energy Principle: A new strategy for modeling Personalities as complex systems", Bibliography!F:F, 0), 1), "CB5T+Free Energy Principle")</f>
         <v>CB5T+Free Energy Principle</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="29" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="29" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
@@ -27633,34 +27795,34 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="41" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B12" s="27" t="str">
         <f xml:space="preserve"> HYPERLINK("#'Bibliography'!" &amp; ADDRESS(MATCH("Self-Entropic Broadening Theory: Toward a New Understanding of Self and Behavior Change Informed by Psychedelics and Psychosis", Bibliography!F:F, 0), 1), "SEBT Theory")</f>
         <v>SEBT Theory</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="26" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="31"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="41" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
@@ -27668,10 +27830,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="32" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="32"/>
@@ -27736,25 +27898,25 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="300">
       <c r="B2" s="49" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="270">
       <c r="B3" s="49" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="270">
       <c r="B4" s="49" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="300">
@@ -27764,37 +27926,37 @@
     </row>
     <row r="6" spans="1:2" ht="285">
       <c r="B6" s="45" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="285">
       <c r="B7" s="49" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="300">
       <c r="B8" s="49" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="240">
       <c r="B9" s="49" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="270">
       <c r="B10" s="49" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="345">
       <c r="B11" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="120">
       <c r="B12" s="49" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -27825,54 +27987,54 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="75">
       <c r="A2" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="345">
       <c r="A3" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="225">
       <c r="A5" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" ht="210">
       <c r="A6" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C6" t="e" vm="2">
         <v>#VALUE!</v>
@@ -27880,13 +28042,13 @@
     </row>
     <row r="7" spans="1:4" ht="300">
       <c r="A7" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final commit before presentation (i hope)
</commit_message>
<xml_diff>
--- a/Excel_References.xlsx
+++ b/Excel_References.xlsx
@@ -19708,8 +19708,8 @@
   <dimension ref="A1:S508"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C85" sqref="C85"/>
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>